<commit_message>
Implement PDF report generation (v1).
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,6 +500,211 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>50</v>
+      </c>
+      <c r="I2" t="n">
+        <v>30</v>
+      </c>
+      <c r="J2" t="n">
+        <v>60</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>50</v>
+      </c>
+      <c r="I3" t="n">
+        <v>30</v>
+      </c>
+      <c r="J3" t="n">
+        <v>60</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>50</v>
+      </c>
+      <c r="I4" t="n">
+        <v>30</v>
+      </c>
+      <c r="J4" t="n">
+        <v>60</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>50</v>
+      </c>
+      <c r="I5" t="n">
+        <v>30</v>
+      </c>
+      <c r="J5" t="n">
+        <v>60</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>20</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>50</v>
+      </c>
+      <c r="I6" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" t="n">
+        <v>60</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>20</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement PDF report generation.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,211 +500,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>50</v>
-      </c>
-      <c r="I2" t="n">
-        <v>30</v>
-      </c>
-      <c r="J2" t="n">
-        <v>60</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>20</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>50</v>
-      </c>
-      <c r="I3" t="n">
-        <v>30</v>
-      </c>
-      <c r="J3" t="n">
-        <v>60</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>20</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
-        <v>50</v>
-      </c>
-      <c r="I4" t="n">
-        <v>30</v>
-      </c>
-      <c r="J4" t="n">
-        <v>60</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>20</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="E5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>50</v>
-      </c>
-      <c r="I5" t="n">
-        <v>30</v>
-      </c>
-      <c r="J5" t="n">
-        <v>60</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>20</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>30</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="E6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>50</v>
-      </c>
-      <c r="I6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J6" t="n">
-        <v>60</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>20</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
PDF report formatting updates.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -523,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="I2" t="n">
         <v>30</v>
@@ -535,7 +535,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="M2" t="n">
         <v>0.05</v>

</xml_diff>

<commit_message>
PDF_report formatting update and Literature Manual Download option.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -508,7 +508,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0.25</v>
@@ -529,7 +529,7 @@
         <v>30</v>
       </c>
       <c r="J2" t="n">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
@@ -538,7 +538,7 @@
         <v>0.1</v>
       </c>
       <c r="M2" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plotting and computation changes.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -508,7 +508,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.002</v>
       </c>
       <c r="D2" t="n">
         <v>0.25</v>
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>9.5</v>
+        <v>15</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -526,10 +526,10 @@
         <v>1000</v>
       </c>
       <c r="I2" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J2" t="n">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Clear cache button, Plots in session_state, Pdf unbreakable content formatting, Equation reference.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,47 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>50</v>
+      </c>
+      <c r="J3" t="n">
+        <v>250</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
data input fields change
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,125 +461,43 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Refernce Head</t>
+          <t>Well ID</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Well ID</t>
+          <t>Pumping Rate</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Pumping Rate</t>
+          <t>X-Coordinates</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>X-Coordinates</t>
+          <t>Y-Coordinates</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Y-Coordinates</t>
+          <t>Layer ID</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Layer ID</t>
+          <t>K Value</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>K Value</t>
+          <t>D Value</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>D Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>15</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I2" t="n">
-        <v>50</v>
-      </c>
-      <c r="J2" t="n">
-        <v>250</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>10</v>
-      </c>
-      <c r="F3" t="n">
-        <v>15</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I3" t="n">
-        <v>50</v>
-      </c>
-      <c r="J3" t="n">
-        <v>250</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.01</v>
+          <t>River Stage</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shift River Stage to River tab.
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,6 +500,47 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>50</v>
+      </c>
+      <c r="I2" t="n">
+        <v>250</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M2" t="n">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Drawdown calculation display update
</commit_message>
<xml_diff>
--- a/RBF_sim_input.xlsx
+++ b/RBF_sim_input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,47 +500,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H2" t="n">
-        <v>50</v>
-      </c>
-      <c r="I2" t="n">
-        <v>250</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="M2" t="n">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>